<commit_message>
Eligibility page + data updates
</commit_message>
<xml_diff>
--- a/RelayCarnivalGrids.xlsx
+++ b/RelayCarnivalGrids.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="1840" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1620" yWindow="2080" windowWidth="18640" windowHeight="21100" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Coaches &amp; Clerk" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="81">
   <si>
     <t>Event</t>
   </si>
@@ -382,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1118,11 +1118,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1462,6 +1475,99 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1501,133 +1607,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,116 +1676,47 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1762,26 +1727,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1834,21 +1856,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1861,8 +1877,14 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2162,23 +2184,23 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="125" t="s">
+      <c r="D2" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="127"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="158"/>
     </row>
     <row r="3" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="122"/>
-      <c r="C3" s="124"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="155"/>
       <c r="D3" s="23">
         <v>1</v>
       </c>
@@ -2202,19 +2224,19 @@
       <c r="C4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="128" t="s">
+      <c r="D4" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="130" t="s">
+      <c r="E4" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="130" t="s">
+      <c r="F4" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="147"/>
+      <c r="H4" s="138"/>
     </row>
     <row r="5" spans="2:8" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32">
@@ -2223,11 +2245,11 @@
       <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="129"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="147"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="138"/>
     </row>
     <row r="6" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33">
@@ -2236,19 +2258,19 @@
       <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="134" t="s">
+      <c r="D6" s="146" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="117" t="s">
+      <c r="E6" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="117" t="s">
+      <c r="F6" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="119" t="s">
+      <c r="G6" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="147"/>
+      <c r="H6" s="138"/>
     </row>
     <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34">
@@ -2257,11 +2279,11 @@
       <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="149"/>
+      <c r="F7" s="149"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="138"/>
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="35">
@@ -2282,7 +2304,7 @@
       <c r="G8" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="147"/>
+      <c r="H8" s="138"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="33">
@@ -2291,19 +2313,19 @@
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="146" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="117" t="s">
+      <c r="E9" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="119" t="s">
+      <c r="G9" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="147"/>
+      <c r="H9" s="138"/>
     </row>
     <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="34">
@@ -2312,11 +2334,11 @@
       <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="135"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="138"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="33">
@@ -2325,19 +2347,19 @@
       <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="149" t="s">
+      <c r="D11" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="130" t="s">
+      <c r="E11" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="132" t="s">
+      <c r="G11" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="147"/>
+      <c r="H11" s="138"/>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34">
@@ -2346,11 +2368,11 @@
       <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="150"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="147"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="138"/>
     </row>
     <row r="13" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="31">
@@ -2359,19 +2381,19 @@
       <c r="C13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="141" t="s">
+      <c r="E13" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="143" t="s">
+      <c r="F13" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="147"/>
+      <c r="H13" s="138"/>
     </row>
     <row r="14" spans="2:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="32">
@@ -2380,22 +2402,22 @@
       <c r="C14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="140"/>
-      <c r="E14" s="142"/>
-      <c r="F14" s="144"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="148"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="137"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="139"/>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="159"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="122"/>
     </row>
     <row r="16" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="33">
@@ -2404,19 +2426,19 @@
       <c r="C16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="139" t="s">
+      <c r="D16" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="141" t="s">
+      <c r="E16" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="143" t="s">
+      <c r="F16" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="145" t="s">
+      <c r="G16" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="136"/>
+      <c r="H16" s="131"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="27">
@@ -2425,11 +2447,11 @@
       <c r="C17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="153"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="155"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="137"/>
+      <c r="D17" s="143"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="132"/>
     </row>
     <row r="18" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27">
@@ -2438,11 +2460,11 @@
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="153"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="155"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="137"/>
+      <c r="D18" s="143"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="132"/>
     </row>
     <row r="19" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34">
@@ -2451,11 +2473,11 @@
       <c r="C19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="140"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="144"/>
-      <c r="G19" s="146"/>
-      <c r="H19" s="137"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="119"/>
+      <c r="H19" s="132"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="29">
@@ -2464,19 +2486,19 @@
       <c r="C20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="160" t="s">
+      <c r="D20" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="151" t="s">
+      <c r="E20" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="151" t="s">
+      <c r="F20" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="152" t="s">
+      <c r="G20" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="137"/>
+      <c r="H20" s="132"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="27">
@@ -2485,11 +2507,11 @@
       <c r="C21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="160"/>
-      <c r="E21" s="151"/>
-      <c r="F21" s="151"/>
-      <c r="G21" s="152"/>
-      <c r="H21" s="137"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="132"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="27">
@@ -2498,11 +2520,11 @@
       <c r="C22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="160"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="137"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="141"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="132"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="27">
@@ -2511,11 +2533,11 @@
       <c r="C23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="160"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="152"/>
-      <c r="H23" s="137"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="132"/>
     </row>
     <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="30">
@@ -2524,22 +2546,22 @@
       <c r="C24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="150"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="138"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="126"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="133"/>
     </row>
     <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="159"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="122"/>
     </row>
     <row r="26" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="31">
@@ -2548,19 +2570,19 @@
       <c r="C26" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="139" t="s">
+      <c r="D26" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="130" t="s">
+      <c r="E26" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="130" t="s">
+      <c r="F26" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="130" t="s">
+      <c r="G26" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="132" t="s">
+      <c r="H26" s="127" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2571,11 +2593,11 @@
       <c r="C27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="140"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="133"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="128"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C28" s="19" t="s">
@@ -2587,6 +2609,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H4:H14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B25:H25"/>
@@ -2597,36 +2643,12 @@
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="D20:D24"/>
     <mergeCell ref="H16:H24"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H4:H14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="E20:E24"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="G20:G24"/>
     <mergeCell ref="D16:D19"/>
     <mergeCell ref="E16:E19"/>
     <mergeCell ref="F16:F19"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2641,7 +2663,7 @@
   </sheetPr>
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2656,26 +2678,26 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="186" t="s">
+      <c r="D2" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="188" t="s">
+      <c r="E2" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="190"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="165"/>
     </row>
     <row r="3" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="122"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="187"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="162"/>
       <c r="E3" s="72" t="s">
         <v>47</v>
       </c>
@@ -2696,15 +2718,15 @@
       <c r="C4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="183" t="s">
+      <c r="D4" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="179"/>
-      <c r="F4" s="166" t="s">
+      <c r="E4" s="170"/>
+      <c r="F4" s="185" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="167"/>
-      <c r="H4" s="169" t="s">
+      <c r="G4" s="172"/>
+      <c r="H4" s="173" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2715,11 +2737,11 @@
       <c r="C5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="178"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="182"/>
-      <c r="H5" s="185"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="167"/>
+      <c r="H5" s="174"/>
     </row>
     <row r="6" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53">
@@ -2728,15 +2750,15 @@
       <c r="C6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="183" t="s">
+      <c r="D6" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="161" t="s">
+      <c r="E6" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="163"/>
-      <c r="G6" s="182"/>
-      <c r="H6" s="171"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="167"/>
+      <c r="H6" s="166"/>
     </row>
     <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="55">
@@ -2745,11 +2767,11 @@
       <c r="C7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="177"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="182"/>
-      <c r="H7" s="171"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="167"/>
+      <c r="H7" s="166"/>
     </row>
     <row r="8" spans="2:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="57">
@@ -2758,7 +2780,7 @@
       <c r="C8" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="177"/>
+      <c r="D8" s="175"/>
       <c r="E8" s="74" t="s">
         <v>52</v>
       </c>
@@ -2779,15 +2801,15 @@
       <c r="C9" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="177"/>
-      <c r="E9" s="161" t="s">
+      <c r="D9" s="175"/>
+      <c r="E9" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="163" t="s">
+      <c r="F9" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="182"/>
-      <c r="H9" s="171"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="166"/>
     </row>
     <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="55">
@@ -2796,11 +2818,11 @@
       <c r="C10" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="177"/>
-      <c r="E10" s="161"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="182"/>
-      <c r="H10" s="171"/>
+      <c r="D10" s="175"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="166"/>
     </row>
     <row r="11" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="53">
@@ -2809,11 +2831,11 @@
       <c r="C11" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="177"/>
-      <c r="E11" s="161"/>
-      <c r="F11" s="163"/>
-      <c r="G11" s="182"/>
-      <c r="H11" s="171"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="176"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="166"/>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="55">
@@ -2822,11 +2844,11 @@
       <c r="C12" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="178"/>
-      <c r="E12" s="161"/>
-      <c r="F12" s="163"/>
-      <c r="G12" s="182"/>
-      <c r="H12" s="171"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="176"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="166"/>
     </row>
     <row r="13" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="49">
@@ -2835,19 +2857,19 @@
       <c r="C13" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="183" t="s">
+      <c r="D13" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="161" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="163" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="163" t="s">
+      <c r="E13" s="184" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="176" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="181" t="s">
+      <c r="H13" s="178" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2858,22 +2880,22 @@
       <c r="C14" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="177"/>
-      <c r="E14" s="162"/>
-      <c r="F14" s="164"/>
-      <c r="G14" s="164"/>
-      <c r="H14" s="170"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="186"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="179"/>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="174"/>
-      <c r="D15" s="174"/>
-      <c r="E15" s="175"/>
-      <c r="F15" s="175"/>
-      <c r="G15" s="175"/>
-      <c r="H15" s="176"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="181"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="183"/>
     </row>
     <row r="16" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="63">
@@ -2882,19 +2904,19 @@
       <c r="C16" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="177" t="s">
+      <c r="D16" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="165" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="166" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="166" t="s">
+      <c r="E16" s="190" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="185" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="185" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="169" t="s">
+      <c r="H16" s="173" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2905,11 +2927,11 @@
       <c r="C17" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="177"/>
-      <c r="E17" s="161"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="181"/>
+      <c r="D17" s="175"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="176"/>
+      <c r="G17" s="176"/>
+      <c r="H17" s="178"/>
     </row>
     <row r="18" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="65">
@@ -2918,11 +2940,11 @@
       <c r="C18" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="177"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="181"/>
+      <c r="D18" s="175"/>
+      <c r="E18" s="184"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="178"/>
     </row>
     <row r="19" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="55">
@@ -2931,11 +2953,11 @@
       <c r="C19" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="178"/>
-      <c r="E19" s="161"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="181"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="184"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="178"/>
     </row>
     <row r="20" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="63">
@@ -2944,17 +2966,17 @@
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="177" t="s">
+      <c r="D20" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="161" t="s">
+      <c r="E20" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="163" t="s">
+      <c r="F20" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="182"/>
-      <c r="H20" s="171"/>
+      <c r="G20" s="167"/>
+      <c r="H20" s="166"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="65">
@@ -2963,11 +2985,11 @@
       <c r="C21" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="177"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="171"/>
+      <c r="D21" s="175"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="176"/>
+      <c r="G21" s="167"/>
+      <c r="H21" s="166"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="65">
@@ -2976,11 +2998,11 @@
       <c r="C22" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="177"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="182"/>
-      <c r="H22" s="171"/>
+      <c r="D22" s="175"/>
+      <c r="E22" s="184"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="166"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="65">
@@ -2989,11 +3011,11 @@
       <c r="C23" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="177"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="182"/>
-      <c r="H23" s="171"/>
+      <c r="D23" s="175"/>
+      <c r="E23" s="184"/>
+      <c r="F23" s="176"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="166"/>
     </row>
     <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="67">
@@ -3002,22 +3024,22 @@
       <c r="C24" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="177"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="168"/>
-      <c r="H24" s="172"/>
+      <c r="D24" s="175"/>
+      <c r="E24" s="186"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="189"/>
+      <c r="H24" s="187"/>
     </row>
     <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="173" t="s">
+      <c r="B25" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="175"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="176"/>
+      <c r="C25" s="181"/>
+      <c r="D25" s="181"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="183"/>
     </row>
     <row r="26" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="69">
@@ -3026,15 +3048,15 @@
       <c r="C26" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="177" t="s">
+      <c r="D26" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="179"/>
-      <c r="F26" s="166" t="s">
+      <c r="E26" s="170"/>
+      <c r="F26" s="185" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="167"/>
-      <c r="H26" s="169" t="s">
+      <c r="G26" s="172"/>
+      <c r="H26" s="173" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3045,11 +3067,11 @@
       <c r="C27" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="178"/>
-      <c r="E27" s="180"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="168"/>
-      <c r="H27" s="170"/>
+      <c r="D27" s="169"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="189"/>
+      <c r="H27" s="179"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C28" s="19" t="s">
@@ -3061,23 +3083,11 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G26:G27"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F4:F7"/>
@@ -3094,11 +3104,23 @@
     <mergeCell ref="H16:H19"/>
     <mergeCell ref="D20:D24"/>
     <mergeCell ref="G20:G24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3134,32 +3156,32 @@
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="125" t="s">
+      <c r="D2" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="186" t="s">
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="188" t="s">
+      <c r="J2" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="189"/>
-      <c r="L2" s="189"/>
-      <c r="M2" s="190"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="165"/>
     </row>
     <row r="3" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="122"/>
-      <c r="C3" s="124"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="155"/>
       <c r="D3" s="23">
         <v>1</v>
       </c>
@@ -3175,7 +3197,7 @@
       <c r="H3" s="25">
         <v>5</v>
       </c>
-      <c r="I3" s="187"/>
+      <c r="I3" s="162"/>
       <c r="J3" s="47" t="s">
         <v>47</v>
       </c>
@@ -3196,28 +3218,28 @@
       <c r="C4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="222" t="s">
+      <c r="D4" s="191" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="130" t="s">
+      <c r="E4" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="130" t="s">
+      <c r="F4" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="147"/>
-      <c r="I4" s="213" t="s">
+      <c r="H4" s="138"/>
+      <c r="I4" s="215" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="207"/>
-      <c r="K4" s="199" t="s">
+      <c r="J4" s="209"/>
+      <c r="K4" s="201" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="203"/>
-      <c r="M4" s="193" t="s">
+      <c r="L4" s="205"/>
+      <c r="M4" s="218" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3228,16 +3250,16 @@
       <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="223"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="207"/>
-      <c r="K5" s="199"/>
-      <c r="L5" s="203"/>
-      <c r="M5" s="193"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="208"/>
+      <c r="J5" s="209"/>
+      <c r="K5" s="201"/>
+      <c r="L5" s="205"/>
+      <c r="M5" s="218"/>
     </row>
     <row r="6" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33">
@@ -3246,28 +3268,28 @@
       <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="220" t="s">
+      <c r="D6" s="193" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="117" t="s">
+      <c r="E6" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="117" t="s">
+      <c r="F6" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="119" t="s">
+      <c r="G6" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="147"/>
-      <c r="I6" s="213" t="s">
+      <c r="H6" s="138"/>
+      <c r="I6" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="208" t="s">
+      <c r="J6" s="210" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="199"/>
-      <c r="L6" s="203"/>
-      <c r="M6" s="195"/>
+      <c r="K6" s="201"/>
+      <c r="L6" s="205"/>
+      <c r="M6" s="220"/>
     </row>
     <row r="7" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34">
@@ -3276,16 +3298,16 @@
       <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="221"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="205"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="199"/>
-      <c r="L7" s="203"/>
-      <c r="M7" s="195"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="149"/>
+      <c r="F7" s="149"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="207"/>
+      <c r="J7" s="210"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="205"/>
+      <c r="M7" s="220"/>
     </row>
     <row r="8" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="35">
@@ -3306,10 +3328,10 @@
       <c r="G8" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="147"/>
-      <c r="I8" s="205"/>
-      <c r="J8" s="208"/>
-      <c r="K8" s="199"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="207"/>
+      <c r="J8" s="210"/>
+      <c r="K8" s="201"/>
       <c r="L8" s="10" t="s">
         <v>45</v>
       </c>
@@ -3324,24 +3346,24 @@
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="220" t="s">
+      <c r="D9" s="193" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="117" t="s">
+      <c r="E9" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="119" t="s">
+      <c r="G9" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="147"/>
-      <c r="I9" s="205"/>
-      <c r="J9" s="208"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="203"/>
-      <c r="M9" s="195"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="207"/>
+      <c r="J9" s="210"/>
+      <c r="K9" s="201"/>
+      <c r="L9" s="205"/>
+      <c r="M9" s="220"/>
     </row>
     <row r="10" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="34">
@@ -3350,16 +3372,16 @@
       <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="221"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="147"/>
-      <c r="I10" s="205"/>
-      <c r="J10" s="208"/>
-      <c r="K10" s="199"/>
-      <c r="L10" s="203"/>
-      <c r="M10" s="195"/>
+      <c r="D10" s="194"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="207"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="201"/>
+      <c r="L10" s="205"/>
+      <c r="M10" s="220"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="33">
@@ -3368,24 +3390,24 @@
       <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="217" t="s">
+      <c r="D11" s="195" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="130" t="s">
+      <c r="E11" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="132" t="s">
+      <c r="G11" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="147"/>
-      <c r="I11" s="205"/>
-      <c r="J11" s="208"/>
-      <c r="K11" s="199"/>
-      <c r="L11" s="203"/>
-      <c r="M11" s="195"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="207"/>
+      <c r="J11" s="210"/>
+      <c r="K11" s="201"/>
+      <c r="L11" s="205"/>
+      <c r="M11" s="220"/>
     </row>
     <row r="12" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34">
@@ -3394,16 +3416,16 @@
       <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="218"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="206"/>
-      <c r="J12" s="208"/>
-      <c r="K12" s="199"/>
-      <c r="L12" s="203"/>
-      <c r="M12" s="195"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="208"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="201"/>
+      <c r="L12" s="205"/>
+      <c r="M12" s="220"/>
     </row>
     <row r="13" spans="2:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="31">
@@ -3412,28 +3434,28 @@
       <c r="C13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="219" t="s">
+      <c r="D13" s="197" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="141" t="s">
+      <c r="E13" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="143" t="s">
+      <c r="F13" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="147"/>
-      <c r="I13" s="213" t="s">
+      <c r="H13" s="138"/>
+      <c r="I13" s="215" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="208"/>
-      <c r="K13" s="199"/>
-      <c r="L13" s="199" t="s">
+      <c r="J13" s="210"/>
+      <c r="K13" s="201"/>
+      <c r="L13" s="201" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="193" t="s">
+      <c r="M13" s="218" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3444,32 +3466,32 @@
       <c r="C14" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="214"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="156"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="205"/>
-      <c r="J14" s="209"/>
-      <c r="K14" s="200"/>
-      <c r="L14" s="200"/>
-      <c r="M14" s="194"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="144"/>
+      <c r="F14" s="145"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="207"/>
+      <c r="J14" s="211"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="219"/>
     </row>
     <row r="15" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
-      <c r="M15" s="159"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="122"/>
     </row>
     <row r="16" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="29">
@@ -3478,32 +3500,32 @@
       <c r="C16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="214" t="s">
+      <c r="D16" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="144" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="155" t="s">
+      <c r="F16" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="156" t="s">
+      <c r="G16" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="137"/>
-      <c r="I16" s="205" t="s">
+      <c r="H16" s="132"/>
+      <c r="I16" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="210" t="s">
+      <c r="J16" s="212" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="201" t="s">
+      <c r="K16" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="201" t="s">
+      <c r="L16" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="196" t="s">
+      <c r="M16" s="221" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3514,16 +3536,16 @@
       <c r="C17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="214"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="155"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="205"/>
-      <c r="J17" s="208"/>
-      <c r="K17" s="199"/>
-      <c r="L17" s="199"/>
-      <c r="M17" s="193"/>
+      <c r="D17" s="198"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="132"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="210"/>
+      <c r="K17" s="201"/>
+      <c r="L17" s="201"/>
+      <c r="M17" s="218"/>
     </row>
     <row r="18" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27">
@@ -3532,16 +3554,16 @@
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="214"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="155"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="137"/>
-      <c r="I18" s="205"/>
-      <c r="J18" s="208"/>
-      <c r="K18" s="199"/>
-      <c r="L18" s="199"/>
-      <c r="M18" s="193"/>
+      <c r="D18" s="198"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="207"/>
+      <c r="J18" s="210"/>
+      <c r="K18" s="201"/>
+      <c r="L18" s="201"/>
+      <c r="M18" s="218"/>
     </row>
     <row r="19" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34">
@@ -3550,16 +3572,16 @@
       <c r="C19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="215"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="144"/>
-      <c r="G19" s="146"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="208"/>
-      <c r="K19" s="199"/>
-      <c r="L19" s="199"/>
-      <c r="M19" s="193"/>
+      <c r="D19" s="199"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="119"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="208"/>
+      <c r="J19" s="210"/>
+      <c r="K19" s="201"/>
+      <c r="L19" s="201"/>
+      <c r="M19" s="218"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="29">
@@ -3568,26 +3590,26 @@
       <c r="C20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="216" t="s">
+      <c r="D20" s="200" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="151" t="s">
+      <c r="E20" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="151" t="s">
+      <c r="F20" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="152" t="s">
+      <c r="G20" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="137"/>
-      <c r="I20" s="205" t="s">
+      <c r="H20" s="132"/>
+      <c r="I20" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="208"/>
-      <c r="K20" s="199"/>
-      <c r="L20" s="203"/>
-      <c r="M20" s="195"/>
+      <c r="J20" s="210"/>
+      <c r="K20" s="201"/>
+      <c r="L20" s="205"/>
+      <c r="M20" s="220"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="27">
@@ -3596,16 +3618,16 @@
       <c r="C21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="216"/>
-      <c r="E21" s="151"/>
-      <c r="F21" s="151"/>
-      <c r="G21" s="152"/>
-      <c r="H21" s="137"/>
-      <c r="I21" s="205"/>
-      <c r="J21" s="208"/>
-      <c r="K21" s="199"/>
-      <c r="L21" s="203"/>
-      <c r="M21" s="195"/>
+      <c r="D21" s="200"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="132"/>
+      <c r="I21" s="207"/>
+      <c r="J21" s="210"/>
+      <c r="K21" s="201"/>
+      <c r="L21" s="205"/>
+      <c r="M21" s="220"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="27">
@@ -3614,16 +3636,16 @@
       <c r="C22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="216"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="137"/>
-      <c r="I22" s="205"/>
-      <c r="J22" s="208"/>
-      <c r="K22" s="199"/>
-      <c r="L22" s="203"/>
-      <c r="M22" s="195"/>
+      <c r="D22" s="200"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="141"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="132"/>
+      <c r="I22" s="207"/>
+      <c r="J22" s="210"/>
+      <c r="K22" s="201"/>
+      <c r="L22" s="205"/>
+      <c r="M22" s="220"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="27">
@@ -3632,16 +3654,16 @@
       <c r="C23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="216"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="152"/>
-      <c r="H23" s="137"/>
-      <c r="I23" s="205"/>
-      <c r="J23" s="208"/>
-      <c r="K23" s="199"/>
-      <c r="L23" s="203"/>
-      <c r="M23" s="195"/>
+      <c r="D23" s="200"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="210"/>
+      <c r="K23" s="201"/>
+      <c r="L23" s="205"/>
+      <c r="M23" s="220"/>
     </row>
     <row r="24" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="30">
@@ -3650,32 +3672,32 @@
       <c r="C24" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="216"/>
-      <c r="E24" s="151"/>
-      <c r="F24" s="151"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="137"/>
-      <c r="I24" s="205"/>
-      <c r="J24" s="209"/>
-      <c r="K24" s="200"/>
-      <c r="L24" s="204"/>
-      <c r="M24" s="198"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="141"/>
+      <c r="F24" s="141"/>
+      <c r="G24" s="142"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="207"/>
+      <c r="J24" s="211"/>
+      <c r="K24" s="202"/>
+      <c r="L24" s="206"/>
+      <c r="M24" s="223"/>
     </row>
     <row r="25" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="158"/>
-      <c r="K25" s="158"/>
-      <c r="L25" s="158"/>
-      <c r="M25" s="159"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="121"/>
+      <c r="K25" s="121"/>
+      <c r="L25" s="121"/>
+      <c r="M25" s="122"/>
     </row>
     <row r="26" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="26">
@@ -3684,30 +3706,30 @@
       <c r="C26" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="214" t="s">
+      <c r="D26" s="198" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="151" t="s">
+      <c r="E26" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="151" t="s">
+      <c r="F26" s="141" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="151" t="s">
+      <c r="G26" s="141" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="152" t="s">
+      <c r="H26" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="205" t="s">
+      <c r="I26" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="211"/>
-      <c r="K26" s="201" t="s">
+      <c r="J26" s="213"/>
+      <c r="K26" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="L26" s="191"/>
-      <c r="M26" s="196" t="s">
+      <c r="L26" s="216"/>
+      <c r="M26" s="221" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3718,16 +3740,16 @@
       <c r="C27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="215"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="133"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="212"/>
-      <c r="K27" s="202"/>
-      <c r="L27" s="192"/>
-      <c r="M27" s="197"/>
+      <c r="D27" s="199"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="208"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="204"/>
+      <c r="L27" s="217"/>
+      <c r="M27" s="222"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C28" s="19" t="s">
@@ -3739,6 +3761,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="I6:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="K4:K14"/>
+    <mergeCell ref="K16:K24"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J14"/>
+    <mergeCell ref="J16:J24"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:H2"/>
@@ -3755,58 +3829,6 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="K4:K14"/>
-    <mergeCell ref="K16:K24"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J14"/>
-    <mergeCell ref="J16:J24"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="I6:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3837,25 +3859,25 @@
   <sheetData>
     <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="186" t="s">
+      <c r="D2" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="241" t="s">
+      <c r="E2" s="224" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="242"/>
-      <c r="G2" s="243"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="226"/>
     </row>
     <row r="3" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="122"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="187"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="162"/>
       <c r="E3" s="47" t="s">
         <v>47</v>
       </c>
@@ -3873,12 +3895,12 @@
       <c r="C4" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="228" t="s">
+      <c r="D4" s="231" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="77"/>
       <c r="F4" s="78"/>
-      <c r="G4" s="226" t="s">
+      <c r="G4" s="229" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3889,10 +3911,10 @@
       <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="230"/>
+      <c r="D5" s="233"/>
       <c r="E5" s="79"/>
       <c r="F5" s="80"/>
-      <c r="G5" s="227"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="96">
@@ -3901,10 +3923,10 @@
       <c r="C6" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="228" t="s">
+      <c r="D6" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="231" t="s">
+      <c r="E6" s="234" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="80"/>
@@ -3917,8 +3939,8 @@
       <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="229"/>
-      <c r="E7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="235"/>
       <c r="F7" s="82"/>
       <c r="G7" s="83"/>
     </row>
@@ -3929,8 +3951,8 @@
       <c r="C8" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="229"/>
-      <c r="E8" s="232"/>
+      <c r="D8" s="232"/>
+      <c r="E8" s="235"/>
       <c r="F8" s="8" t="s">
         <v>58</v>
       </c>
@@ -3945,8 +3967,8 @@
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="229"/>
-      <c r="E9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="235"/>
       <c r="F9" s="78"/>
       <c r="G9" s="81"/>
     </row>
@@ -3957,8 +3979,8 @@
       <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="229"/>
-      <c r="E10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="235"/>
       <c r="F10" s="80"/>
       <c r="G10" s="84"/>
     </row>
@@ -3969,8 +3991,8 @@
       <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="229"/>
-      <c r="E11" s="232"/>
+      <c r="D11" s="232"/>
+      <c r="E11" s="235"/>
       <c r="F11" s="80"/>
       <c r="G11" s="84"/>
     </row>
@@ -3981,8 +4003,8 @@
       <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="230"/>
-      <c r="E12" s="232"/>
+      <c r="D12" s="233"/>
+      <c r="E12" s="235"/>
       <c r="F12" s="82"/>
       <c r="G12" s="83"/>
     </row>
@@ -3993,14 +4015,14 @@
       <c r="C13" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="228" t="s">
+      <c r="D13" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="232"/>
-      <c r="F13" s="239" t="s">
+      <c r="E13" s="235"/>
+      <c r="F13" s="242" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="226" t="s">
+      <c r="G13" s="229" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4011,20 +4033,20 @@
       <c r="C14" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="230"/>
-      <c r="E14" s="233"/>
-      <c r="F14" s="240"/>
-      <c r="G14" s="227"/>
+      <c r="D14" s="233"/>
+      <c r="E14" s="236"/>
+      <c r="F14" s="243"/>
+      <c r="G14" s="230"/>
     </row>
     <row r="15" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="159"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="122"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="88">
@@ -4033,16 +4055,16 @@
       <c r="C16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="228" t="s">
+      <c r="D16" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="231" t="s">
+      <c r="E16" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="234" t="s">
+      <c r="F16" s="237" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="224" t="s">
+      <c r="G16" s="227" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4053,10 +4075,10 @@
       <c r="C17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="229"/>
-      <c r="E17" s="232"/>
-      <c r="F17" s="235"/>
-      <c r="G17" s="237"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="235"/>
+      <c r="F17" s="238"/>
+      <c r="G17" s="240"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="27">
@@ -4065,10 +4087,10 @@
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="229"/>
-      <c r="E18" s="232"/>
-      <c r="F18" s="235"/>
-      <c r="G18" s="237"/>
+      <c r="D18" s="232"/>
+      <c r="E18" s="235"/>
+      <c r="F18" s="238"/>
+      <c r="G18" s="240"/>
     </row>
     <row r="19" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34">
@@ -4077,10 +4099,10 @@
       <c r="C19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="230"/>
-      <c r="E19" s="232"/>
-      <c r="F19" s="236"/>
-      <c r="G19" s="238"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="235"/>
+      <c r="F19" s="239"/>
+      <c r="G19" s="241"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="88">
@@ -4089,10 +4111,10 @@
       <c r="C20" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="228" t="s">
+      <c r="D20" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="232"/>
+      <c r="E20" s="235"/>
       <c r="F20" s="78"/>
       <c r="G20" s="81"/>
     </row>
@@ -4103,8 +4125,8 @@
       <c r="C21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="229"/>
-      <c r="E21" s="232"/>
+      <c r="D21" s="232"/>
+      <c r="E21" s="235"/>
       <c r="F21" s="80"/>
       <c r="G21" s="84"/>
     </row>
@@ -4115,8 +4137,8 @@
       <c r="C22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="229"/>
-      <c r="E22" s="232"/>
+      <c r="D22" s="232"/>
+      <c r="E22" s="235"/>
       <c r="F22" s="80"/>
       <c r="G22" s="84"/>
     </row>
@@ -4127,8 +4149,8 @@
       <c r="C23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="229"/>
-      <c r="E23" s="232"/>
+      <c r="D23" s="232"/>
+      <c r="E23" s="235"/>
       <c r="F23" s="80"/>
       <c r="G23" s="84"/>
     </row>
@@ -4139,20 +4161,20 @@
       <c r="C24" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="230"/>
-      <c r="E24" s="233"/>
+      <c r="D24" s="233"/>
+      <c r="E24" s="236"/>
       <c r="F24" s="85"/>
       <c r="G24" s="86"/>
     </row>
     <row r="25" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="159"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="122"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="90">
@@ -4161,12 +4183,12 @@
       <c r="C26" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="228" t="s">
+      <c r="D26" s="231" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="224" t="s">
+      <c r="G26" s="227" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4177,10 +4199,10 @@
       <c r="C27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="230"/>
+      <c r="D27" s="233"/>
       <c r="E27" s="76"/>
       <c r="F27" s="75"/>
-      <c r="G27" s="225"/>
+      <c r="G27" s="228"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C28" s="19" t="s">
@@ -4192,6 +4214,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E6:E14"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D12"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -4208,10 +4234,6 @@
     <mergeCell ref="D16:D19"/>
     <mergeCell ref="F16:F19"/>
     <mergeCell ref="G16:G19"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E6:E14"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4226,8 +4248,8 @@
   </sheetPr>
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:K87"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4258,24 +4280,24 @@
       <c r="N1" s="245"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="244" t="s">
+      <c r="A2" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="244"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="F2" s="244" t="s">
+      <c r="B2" s="246"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="246"/>
+      <c r="F2" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="K2" s="244" t="s">
+      <c r="G2" s="246"/>
+      <c r="H2" s="246"/>
+      <c r="I2" s="246"/>
+      <c r="K2" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
+      <c r="L2" s="246"/>
+      <c r="M2" s="246"/>
+      <c r="N2" s="246"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F3" s="100"/>
@@ -4285,27 +4307,27 @@
       <c r="A4" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="250" t="s">
+      <c r="B4" s="244" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="250"/>
-      <c r="D4" s="250"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
       <c r="F4" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="250" t="s">
+      <c r="G4" s="244" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="250"/>
-      <c r="I4" s="250"/>
+      <c r="H4" s="244"/>
+      <c r="I4" s="244"/>
       <c r="K4" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="250" t="s">
+      <c r="L4" s="244" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="250"/>
-      <c r="N4" s="250"/>
+      <c r="M4" s="244"/>
+      <c r="N4" s="244"/>
     </row>
     <row r="5" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="114">
@@ -4419,29 +4441,41 @@
       <c r="A8" s="114">
         <v>6</v>
       </c>
-      <c r="B8" s="107"/>
+      <c r="B8" s="107" t="s">
+        <v>68</v>
+      </c>
       <c r="C8" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="107"/>
+      <c r="D8" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E8" s="116"/>
       <c r="F8" s="114">
         <v>6</v>
       </c>
-      <c r="G8" s="107"/>
+      <c r="G8" s="107" t="s">
+        <v>68</v>
+      </c>
       <c r="H8" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="107"/>
+      <c r="I8" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="J8" s="116"/>
       <c r="K8" s="114">
         <v>6</v>
       </c>
-      <c r="L8" s="107"/>
+      <c r="L8" s="107" t="s">
+        <v>68</v>
+      </c>
       <c r="M8" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="107"/>
+      <c r="N8" s="107" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="114">
@@ -4964,20 +4998,20 @@
       <c r="K26" s="245"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="244" t="s">
+      <c r="A27" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="244"/>
-      <c r="C27" s="244"/>
-      <c r="D27" s="244"/>
-      <c r="E27" s="244"/>
-      <c r="G27" s="244" t="s">
+      <c r="B27" s="246"/>
+      <c r="C27" s="246"/>
+      <c r="D27" s="246"/>
+      <c r="E27" s="246"/>
+      <c r="G27" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="244"/>
-      <c r="I27" s="244"/>
-      <c r="J27" s="244"/>
-      <c r="K27" s="244"/>
+      <c r="H27" s="246"/>
+      <c r="I27" s="246"/>
+      <c r="J27" s="246"/>
+      <c r="K27" s="246"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G28" s="100"/>
@@ -4986,21 +5020,21 @@
       <c r="A29" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="250" t="s">
+      <c r="B29" s="244" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="250"/>
-      <c r="D29" s="250"/>
-      <c r="E29" s="250"/>
+      <c r="C29" s="244"/>
+      <c r="D29" s="244"/>
+      <c r="E29" s="244"/>
       <c r="G29" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="250" t="s">
+      <c r="H29" s="244" t="s">
         <v>67</v>
       </c>
-      <c r="I29" s="250"/>
-      <c r="J29" s="250"/>
-      <c r="K29" s="250"/>
+      <c r="I29" s="244"/>
+      <c r="J29" s="244"/>
+      <c r="K29" s="244"/>
     </row>
     <row r="30" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="114">
@@ -5331,21 +5365,21 @@
       <c r="Q49" s="101"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A50" s="244" t="s">
+      <c r="A50" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="244"/>
-      <c r="C50" s="244"/>
-      <c r="D50" s="244"/>
-      <c r="E50" s="244"/>
-      <c r="F50" s="244"/>
-      <c r="G50" s="244"/>
-      <c r="H50" s="244"/>
-      <c r="I50" s="244"/>
-      <c r="J50" s="244"/>
-      <c r="K50" s="244"/>
-      <c r="L50" s="244"/>
-      <c r="M50" s="244"/>
+      <c r="B50" s="246"/>
+      <c r="C50" s="246"/>
+      <c r="D50" s="246"/>
+      <c r="E50" s="246"/>
+      <c r="F50" s="246"/>
+      <c r="G50" s="246"/>
+      <c r="H50" s="246"/>
+      <c r="I50" s="246"/>
+      <c r="J50" s="246"/>
+      <c r="K50" s="246"/>
+      <c r="L50" s="246"/>
+      <c r="M50" s="246"/>
       <c r="N50" s="102"/>
       <c r="O50" s="102"/>
       <c r="P50" s="102"/>
@@ -5359,24 +5393,24 @@
       <c r="A52" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="248" t="s">
+      <c r="B52" s="249" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="249"/>
-      <c r="D52" s="249"/>
-      <c r="E52" s="249"/>
-      <c r="F52" s="248" t="s">
+      <c r="C52" s="250"/>
+      <c r="D52" s="250"/>
+      <c r="E52" s="250"/>
+      <c r="F52" s="249" t="s">
         <v>73</v>
       </c>
-      <c r="G52" s="249"/>
-      <c r="H52" s="249"/>
-      <c r="I52" s="249"/>
-      <c r="J52" s="248" t="s">
+      <c r="G52" s="250"/>
+      <c r="H52" s="250"/>
+      <c r="I52" s="250"/>
+      <c r="J52" s="249" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="249"/>
-      <c r="L52" s="249"/>
-      <c r="M52" s="249"/>
+      <c r="K52" s="250"/>
+      <c r="L52" s="250"/>
+      <c r="M52" s="250"/>
     </row>
     <row r="53" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="107" t="s">
@@ -5685,138 +5719,174 @@
       <c r="A62" s="107">
         <v>10</v>
       </c>
-      <c r="B62" s="110"/>
-      <c r="C62" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D62" s="107"/>
+      <c r="B62" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="107"/>
+      <c r="D62" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E62" s="111"/>
-      <c r="F62" s="110"/>
-      <c r="G62" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H62" s="107"/>
+      <c r="F62" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="107"/>
+      <c r="H62" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I62" s="111"/>
-      <c r="J62" s="110"/>
-      <c r="K62" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L62" s="107"/>
+      <c r="J62" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K62" s="107"/>
+      <c r="L62" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M62" s="111"/>
     </row>
     <row r="63" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="107">
         <v>11</v>
       </c>
-      <c r="B63" s="110"/>
-      <c r="C63" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D63" s="107"/>
+      <c r="B63" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="107"/>
+      <c r="D63" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E63" s="111"/>
-      <c r="F63" s="110"/>
-      <c r="G63" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H63" s="107"/>
+      <c r="F63" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" s="107"/>
+      <c r="H63" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I63" s="111"/>
-      <c r="J63" s="110"/>
-      <c r="K63" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L63" s="107"/>
+      <c r="J63" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K63" s="107"/>
+      <c r="L63" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M63" s="111"/>
     </row>
     <row r="64" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="107">
         <v>12</v>
       </c>
-      <c r="B64" s="110"/>
-      <c r="C64" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D64" s="107"/>
+      <c r="B64" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="107"/>
+      <c r="D64" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E64" s="111"/>
-      <c r="F64" s="110"/>
-      <c r="G64" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H64" s="107"/>
+      <c r="F64" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G64" s="107"/>
+      <c r="H64" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I64" s="111"/>
-      <c r="J64" s="110"/>
-      <c r="K64" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L64" s="107"/>
+      <c r="J64" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K64" s="107"/>
+      <c r="L64" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M64" s="111"/>
     </row>
     <row r="65" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="107">
         <v>13</v>
       </c>
-      <c r="B65" s="110"/>
-      <c r="C65" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" s="107"/>
+      <c r="B65" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="107"/>
+      <c r="D65" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E65" s="111"/>
-      <c r="F65" s="110"/>
-      <c r="G65" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H65" s="107"/>
+      <c r="F65" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G65" s="107"/>
+      <c r="H65" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I65" s="111"/>
-      <c r="J65" s="110"/>
-      <c r="K65" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L65" s="107"/>
+      <c r="J65" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K65" s="107"/>
+      <c r="L65" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M65" s="111"/>
     </row>
     <row r="66" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="107">
         <v>14</v>
       </c>
-      <c r="B66" s="110"/>
-      <c r="C66" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D66" s="107"/>
+      <c r="B66" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="107"/>
+      <c r="D66" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E66" s="111"/>
-      <c r="F66" s="110"/>
-      <c r="G66" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H66" s="107"/>
+      <c r="F66" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G66" s="107"/>
+      <c r="H66" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I66" s="111"/>
-      <c r="J66" s="110"/>
-      <c r="K66" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L66" s="107"/>
+      <c r="J66" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K66" s="107"/>
+      <c r="L66" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M66" s="111"/>
     </row>
     <row r="67" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="107">
         <v>15</v>
       </c>
-      <c r="B67" s="110"/>
-      <c r="C67" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="D67" s="107"/>
+      <c r="B67" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" s="107"/>
+      <c r="D67" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="E67" s="111"/>
-      <c r="F67" s="110"/>
-      <c r="G67" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="H67" s="107"/>
+      <c r="F67" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67" s="107"/>
+      <c r="H67" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="I67" s="111"/>
-      <c r="J67" s="110"/>
-      <c r="K67" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="L67" s="107"/>
+      <c r="J67" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K67" s="107"/>
+      <c r="L67" s="107" t="s">
+        <v>69</v>
+      </c>
       <c r="M67" s="111"/>
     </row>
     <row r="68" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,19 +6168,19 @@
       <c r="Q77" s="101"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="244" t="s">
+      <c r="A78" s="246" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="244"/>
-      <c r="C78" s="244"/>
-      <c r="D78" s="244"/>
-      <c r="E78" s="244"/>
-      <c r="F78" s="244"/>
-      <c r="G78" s="244"/>
-      <c r="H78" s="244"/>
-      <c r="I78" s="244"/>
-      <c r="J78" s="244"/>
-      <c r="K78" s="244"/>
+      <c r="B78" s="246"/>
+      <c r="C78" s="246"/>
+      <c r="D78" s="246"/>
+      <c r="E78" s="246"/>
+      <c r="F78" s="246"/>
+      <c r="G78" s="246"/>
+      <c r="H78" s="246"/>
+      <c r="I78" s="246"/>
+      <c r="J78" s="246"/>
+      <c r="K78" s="246"/>
       <c r="L78" s="102"/>
       <c r="M78" s="102"/>
       <c r="N78" s="102"/>
@@ -6126,30 +6196,30 @@
       <c r="A80" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="246" t="s">
+      <c r="B80" s="247" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="247"/>
+      <c r="C80" s="248"/>
       <c r="E80" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="F80" s="246" t="s">
+      <c r="F80" s="247" t="s">
         <v>73</v>
       </c>
-      <c r="G80" s="247"/>
+      <c r="G80" s="248"/>
       <c r="I80" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="J80" s="246" t="s">
+      <c r="J80" s="247" t="s">
         <v>73</v>
       </c>
-      <c r="K80" s="247"/>
+      <c r="K80" s="248"/>
     </row>
     <row r="81" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="106">
         <v>5</v>
       </c>
-      <c r="B81" s="104" t="s">
+      <c r="B81" s="253" t="s">
         <v>68</v>
       </c>
       <c r="C81" s="104" t="s">
@@ -6158,7 +6228,7 @@
       <c r="E81" s="106">
         <v>5</v>
       </c>
-      <c r="F81" s="104" t="s">
+      <c r="F81" s="253" t="s">
         <v>68</v>
       </c>
       <c r="G81" s="104" t="s">
@@ -6167,7 +6237,7 @@
       <c r="I81" s="106">
         <v>5</v>
       </c>
-      <c r="J81" s="104" t="s">
+      <c r="J81" s="253" t="s">
         <v>68</v>
       </c>
       <c r="K81" s="104" t="s">
@@ -6178,195 +6248,160 @@
       <c r="A82" s="106">
         <v>10</v>
       </c>
-      <c r="B82" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C82" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B82" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C82" s="251"/>
       <c r="E82" s="106">
         <v>10</v>
       </c>
-      <c r="F82" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G82" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F82" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G82" s="251"/>
       <c r="I82" s="106">
         <v>10</v>
       </c>
-      <c r="J82" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K82" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J82" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K82" s="251"/>
     </row>
     <row r="83" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="106">
         <v>11</v>
       </c>
-      <c r="B83" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B83" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="251"/>
       <c r="E83" s="106">
         <v>11</v>
       </c>
-      <c r="F83" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G83" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F83" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G83" s="251"/>
       <c r="I83" s="106">
         <v>11</v>
       </c>
-      <c r="J83" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K83" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J83" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K83" s="251"/>
     </row>
     <row r="84" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="106">
         <v>12</v>
       </c>
-      <c r="B84" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B84" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="251"/>
       <c r="E84" s="106">
         <v>12</v>
       </c>
-      <c r="F84" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G84" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F84" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G84" s="251"/>
       <c r="I84" s="106">
         <v>12</v>
       </c>
-      <c r="J84" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K84" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J84" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K84" s="251"/>
     </row>
     <row r="85" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="106">
         <v>13</v>
       </c>
-      <c r="B85" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C85" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B85" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" s="251"/>
       <c r="E85" s="106">
         <v>13</v>
       </c>
-      <c r="F85" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G85" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F85" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G85" s="251"/>
       <c r="I85" s="106">
         <v>13</v>
       </c>
-      <c r="J85" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K85" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J85" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K85" s="251"/>
     </row>
     <row r="86" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="106">
         <v>14</v>
       </c>
-      <c r="B86" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B86" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C86" s="251"/>
       <c r="E86" s="106">
         <v>14</v>
       </c>
-      <c r="F86" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F86" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G86" s="251"/>
       <c r="I86" s="106">
         <v>14</v>
       </c>
-      <c r="J86" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K86" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J86" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K86" s="251"/>
     </row>
     <row r="87" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="106">
         <v>15</v>
       </c>
-      <c r="B87" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="C87" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="B87" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="C87" s="251"/>
       <c r="E87" s="106">
         <v>15</v>
       </c>
-      <c r="F87" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="G87" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="F87" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="G87" s="251"/>
       <c r="I87" s="106">
         <v>15</v>
       </c>
-      <c r="J87" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="K87" s="104" t="s">
-        <v>69</v>
-      </c>
+      <c r="J87" s="252" t="s">
+        <v>52</v>
+      </c>
+      <c r="K87" s="251"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="L4:N4"/>
+  <mergeCells count="45">
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
     <mergeCell ref="A78:K78"/>
     <mergeCell ref="A49:M49"/>
     <mergeCell ref="A50:M50"/>
@@ -6377,6 +6412,23 @@
     <mergeCell ref="F52:I52"/>
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="B52:E52"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>